<commit_message>
The minutes to be loaded to the database
</commit_message>
<xml_diff>
--- a/v/code/minutes.xlsx
+++ b/v/code/minutes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mutall projects\tracker\v\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A79E49F0-8B0B-4C1F-9598-B8DB2BE9ABC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{06AEBACC-E535-4E40-A2B4-28DC1F209059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Minutes" sheetId="1" r:id="rId1"/>
+    <sheet name="minutes" sheetId="1" r:id="rId1"/>
     <sheet name="Contributions" sheetId="2" r:id="rId2"/>
     <sheet name="workplan2024" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="498">
   <si>
     <t>Project</t>
   </si>
@@ -727,15 +727,6 @@
     <t>Add rank summary</t>
   </si>
   <si>
-    <t>upload to the server the school system(talk to peter)</t>
-  </si>
-  <si>
-    <t>Complete the 'edit-score' option - by implementing the save method using the questionnaire library</t>
-  </si>
-  <si>
-    <t>Students graduation. - Consider the fact that students graduate from one grade to another after an year by creating new progressions.</t>
-  </si>
-  <si>
     <t>Report progress on bundler Webpack see if it solves the problem we had</t>
   </si>
   <si>
@@ -1068,6 +1059,474 @@
   </si>
   <si>
     <t>OCR/ Handwritting</t>
+  </si>
+  <si>
+    <t>Nelson button shows the docs site</t>
+  </si>
+  <si>
+    <t>Boundary Conflict resolution.</t>
+  </si>
+  <si>
+    <t>Work on the timetable application to ensure that the minutes of the days presenter are opened by default and the minute that was opened is highlighted on the navigation pannel</t>
+  </si>
+  <si>
+    <t>Finalize the general registration by getting the business detils from the user</t>
+  </si>
+  <si>
+    <t>Work on the version 2 form to make it more responsive to user action and ready for data collection using the get_value method</t>
+  </si>
+  <si>
+    <t>Work on the usage of the registration to ensure that the relevant message is shown given the presence or absence of a user</t>
+  </si>
+  <si>
+    <t>Document the registration system</t>
+  </si>
+  <si>
+    <t>Work on the dialog functionality</t>
+  </si>
+  <si>
+    <t>Implement the form preparation method (Add error reporting and required marks on inputs)</t>
+  </si>
+  <si>
+    <t>Clear all the errors on input</t>
+  </si>
+  <si>
+    <t>Do extensive tests on the dialog</t>
+  </si>
+  <si>
+    <t>Document the dialog class</t>
+  </si>
+  <si>
+    <t>Test the code we developed as a group</t>
+  </si>
+  <si>
+    <t>Start writing the rent qury</t>
+  </si>
+  <si>
+    <t>Work on the mutall_rental loan query</t>
+  </si>
+  <si>
+    <t>Sketch the expected results of the loan query</t>
+  </si>
+  <si>
+    <t>Help Anne to implement the search functionality in the makubaliano document</t>
+  </si>
+  <si>
+    <t>Work with Muli to get images from the database to his webpage</t>
+  </si>
+  <si>
+    <t>Test the mother.ts project and ensure it works for all radio forms i.e., registration, images and sheetjs(MW)</t>
+  </si>
+  <si>
+    <t>Develop a php application template and in that template work on implementing the login and messaging functionality(SK)</t>
+  </si>
+  <si>
+    <t>Ensure that the get_value method of the view works given the new form design constrains</t>
+  </si>
+  <si>
+    <t>Think about the set_value method of the view</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>3.1.4</t>
+  </si>
+  <si>
+    <t>Add an onclick event listener to display images on the  right had panel</t>
+  </si>
+  <si>
+    <t>Highlight the clicked item</t>
+  </si>
+  <si>
+    <t>Design a query for extracting client contract details</t>
+  </si>
+  <si>
+    <t>Add a facility for tracking customer deposits</t>
+  </si>
+  <si>
+    <t>Create Balansys Transcription database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display the database on metavisuo   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design a transcription form that matches its database  </t>
+  </si>
+  <si>
+    <t>show the size of the image for security reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the image large to fit the image area  </t>
+  </si>
+  <si>
+    <t>Produce invoices on request</t>
+  </si>
+  <si>
+    <t>Do research on CORS Origin policy</t>
+  </si>
+  <si>
+    <t>Report on progress</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>Get electicity data from mutall_rental database.</t>
+  </si>
+  <si>
+    <t>Sketch the data ill be collecting.</t>
+  </si>
+  <si>
+    <t>Create a query for retrieving the data.</t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download images that represent items on the workplan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design a webpage the and illustrates all the services available from your cybercafe.  </t>
+  </si>
+  <si>
+    <t>Study inturn registration form and use it on mutall rental for new client registration</t>
+  </si>
+  <si>
+    <t>Work with Ann to improve mutall rental</t>
+  </si>
+  <si>
+    <t>Improve mutall rental to review contracts automatically</t>
+  </si>
+  <si>
+    <t>Customer Deposits</t>
+  </si>
+  <si>
+    <t>Study Mutall Rental data model relationships</t>
+  </si>
+  <si>
+    <t>Report progress on data collection</t>
+  </si>
+  <si>
+    <t>Design a data collection system</t>
+  </si>
+  <si>
+    <t>Get help from Mogaka to display images from the database</t>
+  </si>
+  <si>
+    <t>Display an image using an image tag</t>
+  </si>
+  <si>
+    <t>Get Kibe to help with the receipts transcription interface</t>
+  </si>
+  <si>
+    <t>Change stock taking interface colours</t>
+  </si>
+  <si>
+    <t>Use tabular fomat of data collection on all balansys interfaces</t>
+  </si>
+  <si>
+    <t>Remove place holders on the balansys stock user interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand, Refine and expound on items on the workplan with Mr Muraya   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is exactly the task that Ann and I are supposed to work on  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn how to create a zoom meeting  </t>
+  </si>
+  <si>
+    <t>Learning git hub</t>
+  </si>
+  <si>
+    <t>Learning CMD to help me navigate github</t>
+  </si>
+  <si>
+    <t>Design a new client registration form</t>
+  </si>
+  <si>
+    <t>Get all receipts transcribed on the balansys workbook</t>
+  </si>
+  <si>
+    <t>Merge Mogaka and Kibe's code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loading images to the database  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design a new client registration form    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft a new client registration form on paper  </t>
+  </si>
+  <si>
+    <t>Add a time stamp on uploaded images</t>
+  </si>
+  <si>
+    <t>Document Balansys</t>
+  </si>
+  <si>
+    <t>Develop a software to upload images to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop an android application to save images staight from  phone to db </t>
+  </si>
+  <si>
+    <t>add balansys logo on the top left of all balansys interfaces</t>
+  </si>
+  <si>
+    <t>add the name of the interface in the middle</t>
+  </si>
+  <si>
+    <t>put the names of developers in  the middle grid and add links on their names to their hubs</t>
+  </si>
+  <si>
+    <t>on stock management interface, make the middle grid independent for the sake of phone view</t>
+  </si>
+  <si>
+    <t>make the image on transcription interface large by default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add an onclick event listener on select radio buttons that open a list  </t>
+  </si>
+  <si>
+    <t>fix bug on add row code</t>
+  </si>
+  <si>
+    <t>2.3.2</t>
+  </si>
+  <si>
+    <t>2.3.3</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
+  </si>
+  <si>
+    <t>2.3.5</t>
+  </si>
+  <si>
+    <t>2.3.6</t>
+  </si>
+  <si>
+    <t>2.3.7</t>
+  </si>
+  <si>
+    <t>2.3.8</t>
+  </si>
+  <si>
+    <t>Get clients unique identifiers</t>
+  </si>
+  <si>
+    <t>Get agreement details from db</t>
+  </si>
+  <si>
+    <t>Button event listener</t>
+  </si>
+  <si>
+    <t>Increase image size</t>
+  </si>
+  <si>
+    <t>Mobile view</t>
+  </si>
+  <si>
+    <t>Add the developers to the footer</t>
+  </si>
+  <si>
+    <t>Add a logo</t>
+  </si>
+  <si>
+    <t>Android app for image upload</t>
+  </si>
+  <si>
+    <t>Image upload software</t>
+  </si>
+  <si>
+    <t>Recipts Transcription</t>
+  </si>
+  <si>
+    <t>Investigate on Annes work</t>
+  </si>
+  <si>
+    <t>Work on your work plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove placeholders </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabular layout </t>
+  </si>
+  <si>
+    <t>Transcription interface</t>
+  </si>
+  <si>
+    <t>Style the transcription interface with Munya</t>
+  </si>
+  <si>
+    <t>Db image display</t>
+  </si>
+  <si>
+    <t>Mutall rental contract renewall</t>
+  </si>
+  <si>
+    <t>Client registration mutall rental</t>
+  </si>
+  <si>
+    <t>Cyber web page</t>
+  </si>
+  <si>
+    <t>Get relevant images for your workplan</t>
+  </si>
+  <si>
+    <t>Design transcription dbase</t>
+  </si>
+  <si>
+    <t>Client contract extraction</t>
+  </si>
+  <si>
+    <t>Event listener for image display</t>
+  </si>
+  <si>
+    <t>Get value testing</t>
+  </si>
+  <si>
+    <t>General app template</t>
+  </si>
+  <si>
+    <t>Testing of the flactuate code</t>
+  </si>
+  <si>
+    <t>Display of images form dbase</t>
+  </si>
+  <si>
+    <t>Search functionality in the makubaliano</t>
+  </si>
+  <si>
+    <t>Form preparation on dialog</t>
+  </si>
+  <si>
+    <t>Registration version 2</t>
+  </si>
+  <si>
+    <t>Level 2 registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focus on projects rather </t>
+  </si>
+  <si>
+    <t>Placement letters to embasy</t>
+  </si>
+  <si>
+    <t>Metavisuo debugging</t>
+  </si>
+  <si>
+    <t>Tree walker fo highligting words</t>
+  </si>
+  <si>
+    <t>Key value pair of all data-id fields</t>
+  </si>
+  <si>
+    <t>Add extract data button</t>
+  </si>
+  <si>
+    <t>Mutall rental query</t>
+  </si>
+  <si>
+    <t>Saving data on the serevr</t>
+  </si>
+  <si>
+    <t>Students graduation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Consider the fact that students graduate from one grade to another after an year by creating new progressions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the 'edit-score' option </t>
+  </si>
+  <si>
+    <t>by implementing the save method using the questionnaire library</t>
+  </si>
+  <si>
+    <t>upload to the server the school system</t>
+  </si>
+  <si>
+    <t>(talk to peter)</t>
+  </si>
+  <si>
+    <t>Webpack invesigation</t>
+  </si>
+  <si>
+    <t>Xamp installation documentation</t>
+  </si>
+  <si>
+    <t>Add coments to your code</t>
+  </si>
+  <si>
+    <t>Dialog for user input</t>
+  </si>
+  <si>
+    <t>Develop a structure to hold the query data</t>
+  </si>
+  <si>
+    <t>Xml</t>
+  </si>
+  <si>
+    <t>Return type on save</t>
+  </si>
+  <si>
+    <t>Upload image function</t>
+  </si>
+  <si>
+    <t>Data collection from user</t>
+  </si>
+  <si>
+    <t>Create dialog</t>
+  </si>
+  <si>
+    <t>Work on log out</t>
+  </si>
+  <si>
+    <t>Implement the abstract methods</t>
+  </si>
+  <si>
+    <t>Work on editing a contribution</t>
+  </si>
+  <si>
+    <t>Separation of a contribution from presentation</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Get the data collection from from the html doc</t>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>Folder structure organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metavisuo </t>
+  </si>
+  <si>
+    <t>Mark Identification attributes</t>
+  </si>
+  <si>
+    <t>Errors</t>
   </si>
 </sst>
 </file>
@@ -1400,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F278"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E203" sqref="E203"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F273" sqref="F273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1870,7 @@
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="52.5703125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
   </cols>
@@ -3220,6 +3679,9 @@
         <v>3.2</v>
       </c>
       <c r="D125" t="s">
+        <v>497</v>
+      </c>
+      <c r="E125" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3231,6 +3693,9 @@
         <v>3.3</v>
       </c>
       <c r="D126" t="s">
+        <v>496</v>
+      </c>
+      <c r="E126" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3253,10 +3718,13 @@
         <v>3.5</v>
       </c>
       <c r="D128" t="s">
+        <v>495</v>
+      </c>
+      <c r="E128" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>84</v>
       </c>
@@ -3264,10 +3732,13 @@
         <v>3.6</v>
       </c>
       <c r="D129" t="s">
+        <v>94</v>
+      </c>
+      <c r="E129" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>84</v>
       </c>
@@ -3281,7 +3752,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>84</v>
       </c>
@@ -3292,10 +3763,13 @@
         <v>184</v>
       </c>
       <c r="D131" t="s">
+        <v>494</v>
+      </c>
+      <c r="E131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>84</v>
       </c>
@@ -3306,10 +3780,13 @@
         <v>185</v>
       </c>
       <c r="D132" t="s">
+        <v>493</v>
+      </c>
+      <c r="E132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>84</v>
       </c>
@@ -3320,10 +3797,13 @@
         <v>186</v>
       </c>
       <c r="D133" t="s">
+        <v>492</v>
+      </c>
+      <c r="E133" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>84</v>
       </c>
@@ -3334,10 +3814,13 @@
         <v>187</v>
       </c>
       <c r="D134" t="s">
+        <v>491</v>
+      </c>
+      <c r="E134" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>84</v>
       </c>
@@ -3348,10 +3831,13 @@
         <v>188</v>
       </c>
       <c r="D135" t="s">
+        <v>490</v>
+      </c>
+      <c r="E135" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>84</v>
       </c>
@@ -3362,10 +3848,13 @@
         <v>1.2</v>
       </c>
       <c r="D136" t="s">
+        <v>489</v>
+      </c>
+      <c r="E136" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>84</v>
       </c>
@@ -3376,10 +3865,13 @@
         <v>1.3</v>
       </c>
       <c r="D137" t="s">
+        <v>488</v>
+      </c>
+      <c r="E137" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>85</v>
       </c>
@@ -3387,10 +3879,13 @@
         <v>2.1</v>
       </c>
       <c r="D138" t="s">
+        <v>487</v>
+      </c>
+      <c r="E138" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>85</v>
       </c>
@@ -3401,7 +3896,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>85</v>
       </c>
@@ -3412,7 +3907,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>85</v>
       </c>
@@ -3423,7 +3918,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>85</v>
       </c>
@@ -3431,10 +3926,13 @@
         <v>3.1</v>
       </c>
       <c r="D142" t="s">
+        <v>486</v>
+      </c>
+      <c r="E142" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>85</v>
       </c>
@@ -3442,10 +3940,13 @@
         <v>3.2</v>
       </c>
       <c r="D143" t="s">
+        <v>485</v>
+      </c>
+      <c r="E143" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>85</v>
       </c>
@@ -3453,6 +3954,9 @@
         <v>3.3</v>
       </c>
       <c r="D144" t="s">
+        <v>484</v>
+      </c>
+      <c r="E144" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3464,6 +3968,9 @@
         <v>3.4</v>
       </c>
       <c r="D145" t="s">
+        <v>483</v>
+      </c>
+      <c r="E145" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3475,6 +3982,9 @@
         <v>3.5</v>
       </c>
       <c r="D146" t="s">
+        <v>482</v>
+      </c>
+      <c r="E146" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3508,6 +4018,9 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D149" t="s">
+        <v>481</v>
+      </c>
+      <c r="E149" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3530,6 +4043,9 @@
         <v>5.3</v>
       </c>
       <c r="D151" t="s">
+        <v>480</v>
+      </c>
+      <c r="E151" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3541,6 +4057,9 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D152" t="s">
+        <v>479</v>
+      </c>
+      <c r="E152" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3552,6 +4071,9 @@
         <v>1.2</v>
       </c>
       <c r="D153" t="s">
+        <v>431</v>
+      </c>
+      <c r="E153" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3563,6 +4085,9 @@
         <v>3.1</v>
       </c>
       <c r="D154" t="s">
+        <v>432</v>
+      </c>
+      <c r="E154" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3709,6 +4234,9 @@
         <v>5.4</v>
       </c>
       <c r="D164" t="s">
+        <v>478</v>
+      </c>
+      <c r="E164" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3779,7 +4307,10 @@
         <v>1.3</v>
       </c>
       <c r="D169" t="s">
-        <v>231</v>
+        <v>475</v>
+      </c>
+      <c r="E169" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3793,7 +4324,10 @@
         <v>1.4</v>
       </c>
       <c r="D170" t="s">
-        <v>232</v>
+        <v>473</v>
+      </c>
+      <c r="E170" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3807,7 +4341,10 @@
         <v>1.5</v>
       </c>
       <c r="D171" t="s">
-        <v>233</v>
+        <v>471</v>
+      </c>
+      <c r="E171" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3821,7 +4358,10 @@
         <v>2.1</v>
       </c>
       <c r="D172" t="s">
-        <v>234</v>
+        <v>477</v>
+      </c>
+      <c r="E172" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3835,7 +4375,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D173" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -3846,7 +4386,7 @@
         <v>3.1</v>
       </c>
       <c r="D174" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,7 +4397,7 @@
         <v>3.2</v>
       </c>
       <c r="D175" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,10 +4408,10 @@
         <v>3.3</v>
       </c>
       <c r="D176" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>88</v>
       </c>
@@ -3879,10 +4419,13 @@
         <v>3.4</v>
       </c>
       <c r="D177" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+      <c r="E177" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>88</v>
       </c>
@@ -3890,10 +4433,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D178" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>88</v>
       </c>
@@ -3901,10 +4444,13 @@
         <v>4.2</v>
       </c>
       <c r="D179" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="E179" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>89</v>
       </c>
@@ -3915,7 +4461,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>89</v>
       </c>
@@ -3923,10 +4469,10 @@
         <v>1.2</v>
       </c>
       <c r="D181" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>89</v>
       </c>
@@ -3934,10 +4480,10 @@
         <v>2.1</v>
       </c>
       <c r="D182" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>89</v>
       </c>
@@ -3945,10 +4491,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D183" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>89</v>
       </c>
@@ -3956,10 +4502,10 @@
         <v>3.1</v>
       </c>
       <c r="D184" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>89</v>
       </c>
@@ -3967,10 +4513,10 @@
         <v>3.2</v>
       </c>
       <c r="D185" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>89</v>
       </c>
@@ -3978,10 +4524,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D186" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>89</v>
       </c>
@@ -3989,10 +4535,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D187" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>89</v>
       </c>
@@ -4000,10 +4546,10 @@
         <v>6.1</v>
       </c>
       <c r="D188" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>66</v>
       </c>
@@ -4017,7 +4563,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>90</v>
       </c>
@@ -4028,7 +4574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>90</v>
       </c>
@@ -4036,10 +4582,10 @@
         <v>1.2</v>
       </c>
       <c r="D191" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>90</v>
       </c>
@@ -4047,7 +4593,10 @@
         <v>1.3</v>
       </c>
       <c r="D192" t="s">
-        <v>250</v>
+        <v>468</v>
+      </c>
+      <c r="E192" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4058,7 +4607,10 @@
         <v>1.4</v>
       </c>
       <c r="D193" t="s">
-        <v>251</v>
+        <v>467</v>
+      </c>
+      <c r="E193" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4069,7 +4621,10 @@
         <v>1.5</v>
       </c>
       <c r="D194" t="s">
-        <v>252</v>
+        <v>466</v>
+      </c>
+      <c r="E194" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4080,7 +4635,10 @@
         <v>2.1</v>
       </c>
       <c r="D195" t="s">
-        <v>253</v>
+        <v>465</v>
+      </c>
+      <c r="E195" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4091,7 +4649,10 @@
         <v>3.1</v>
       </c>
       <c r="D196" t="s">
-        <v>254</v>
+        <v>464</v>
+      </c>
+      <c r="E196" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4105,7 +4666,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D197" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4129,11 +4690,14 @@
       <c r="B199">
         <v>91</v>
       </c>
+      <c r="C199">
+        <v>1.3</v>
+      </c>
       <c r="D199" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4143,10 +4707,1061 @@
       <c r="B200">
         <v>91</v>
       </c>
+      <c r="C200">
+        <v>1.4</v>
+      </c>
+      <c r="D200" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>40</v>
+      </c>
       <c r="B201">
         <v>91</v>
+      </c>
+      <c r="C201">
+        <v>1.5</v>
+      </c>
+      <c r="D201" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>40</v>
+      </c>
+      <c r="B202">
+        <v>91</v>
+      </c>
+      <c r="C202">
+        <v>1.6</v>
+      </c>
+      <c r="D202" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>14</v>
+      </c>
+      <c r="B203">
+        <v>93</v>
+      </c>
+      <c r="C203">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D203" t="s">
+        <v>463</v>
+      </c>
+      <c r="E203" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>93</v>
+      </c>
+      <c r="C204">
+        <v>2.1</v>
+      </c>
+      <c r="D204" t="s">
+        <v>462</v>
+      </c>
+      <c r="E204" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>93</v>
+      </c>
+      <c r="C205">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D205" t="s">
+        <v>461</v>
+      </c>
+      <c r="E205" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>93</v>
+      </c>
+      <c r="C206">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D206" t="s">
+        <v>133</v>
+      </c>
+      <c r="E206" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>93</v>
+      </c>
+      <c r="C207">
+        <v>2.4</v>
+      </c>
+      <c r="D207" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>93</v>
+      </c>
+      <c r="C208">
+        <v>3.1</v>
+      </c>
+      <c r="D208" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>93</v>
+      </c>
+      <c r="C209" t="s">
+        <v>365</v>
+      </c>
+      <c r="D209" t="s">
+        <v>460</v>
+      </c>
+      <c r="E209" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>93</v>
+      </c>
+      <c r="C210" t="s">
+        <v>366</v>
+      </c>
+      <c r="D210" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>93</v>
+      </c>
+      <c r="C211" t="s">
+        <v>367</v>
+      </c>
+      <c r="D211" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>93</v>
+      </c>
+      <c r="C212" t="s">
+        <v>368</v>
+      </c>
+      <c r="D212" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>93</v>
+      </c>
+      <c r="C213">
+        <v>3.2</v>
+      </c>
+      <c r="D213" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>93</v>
+      </c>
+      <c r="C214">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D214" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>93</v>
+      </c>
+      <c r="C215">
+        <v>4.2</v>
+      </c>
+      <c r="D215" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>93</v>
+      </c>
+      <c r="C216" t="s">
+        <v>364</v>
+      </c>
+      <c r="D216" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>93</v>
+      </c>
+      <c r="C217">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D217" t="s">
+        <v>459</v>
+      </c>
+      <c r="E217" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>93</v>
+      </c>
+      <c r="C218">
+        <v>5.2</v>
+      </c>
+      <c r="D218" t="s">
+        <v>458</v>
+      </c>
+      <c r="E218" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>93</v>
+      </c>
+      <c r="C219">
+        <v>5.3</v>
+      </c>
+      <c r="D219" t="s">
+        <v>457</v>
+      </c>
+      <c r="E219" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>93</v>
+      </c>
+      <c r="C220">
+        <v>5.4</v>
+      </c>
+      <c r="D220" t="s">
+        <v>456</v>
+      </c>
+      <c r="E220" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>93</v>
+      </c>
+      <c r="C221">
+        <v>5.5</v>
+      </c>
+      <c r="D221" t="s">
+        <v>455</v>
+      </c>
+      <c r="E221" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>93</v>
+      </c>
+      <c r="C222">
+        <v>5.6</v>
+      </c>
+      <c r="D222" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>94</v>
+      </c>
+      <c r="C223">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D223" t="s">
+        <v>454</v>
+      </c>
+      <c r="E223" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>94</v>
+      </c>
+      <c r="C224" t="s">
+        <v>184</v>
+      </c>
+      <c r="D224" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>94</v>
+      </c>
+      <c r="C225">
+        <v>1.2</v>
+      </c>
+      <c r="D225" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>90</v>
+      </c>
+      <c r="B226">
+        <v>94</v>
+      </c>
+      <c r="C226">
+        <v>2.1</v>
+      </c>
+      <c r="D226" t="s">
+        <v>453</v>
+      </c>
+      <c r="E226" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>90</v>
+      </c>
+      <c r="B227">
+        <v>94</v>
+      </c>
+      <c r="C227">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D227" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>88</v>
+      </c>
+      <c r="B228">
+        <v>94</v>
+      </c>
+      <c r="C228">
+        <v>3.1</v>
+      </c>
+      <c r="D228" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>88</v>
+      </c>
+      <c r="B229">
+        <v>94</v>
+      </c>
+      <c r="C229" t="s">
+        <v>365</v>
+      </c>
+      <c r="D229" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>88</v>
+      </c>
+      <c r="B230">
+        <v>94</v>
+      </c>
+      <c r="C230">
+        <v>3.2</v>
+      </c>
+      <c r="D230" t="s">
+        <v>452</v>
+      </c>
+      <c r="E230" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>88</v>
+      </c>
+      <c r="B231">
+        <v>94</v>
+      </c>
+      <c r="C231" t="s">
+        <v>381</v>
+      </c>
+      <c r="D231" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>88</v>
+      </c>
+      <c r="B232">
+        <v>94</v>
+      </c>
+      <c r="C232" t="s">
+        <v>382</v>
+      </c>
+      <c r="D232" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>92</v>
+      </c>
+      <c r="B233">
+        <v>94</v>
+      </c>
+      <c r="C233">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D233" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>92</v>
+      </c>
+      <c r="B234">
+        <v>94</v>
+      </c>
+      <c r="C234">
+        <v>4.2</v>
+      </c>
+      <c r="D234" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>92</v>
+      </c>
+      <c r="B235">
+        <v>94</v>
+      </c>
+      <c r="C235" t="s">
+        <v>364</v>
+      </c>
+      <c r="D235" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>89</v>
+      </c>
+      <c r="B236">
+        <v>94</v>
+      </c>
+      <c r="C236">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D236" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>91</v>
+      </c>
+      <c r="B237">
+        <v>94</v>
+      </c>
+      <c r="C237">
+        <v>6.1</v>
+      </c>
+      <c r="D237" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>95</v>
+      </c>
+      <c r="C238">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D238" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>95</v>
+      </c>
+      <c r="C239" t="s">
+        <v>184</v>
+      </c>
+      <c r="D239" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>95</v>
+      </c>
+      <c r="C240" t="s">
+        <v>185</v>
+      </c>
+      <c r="D240" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>96</v>
+      </c>
+      <c r="C241">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D241" t="s">
+        <v>451</v>
+      </c>
+      <c r="E241" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>96</v>
+      </c>
+      <c r="C242">
+        <v>2.1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>450</v>
+      </c>
+      <c r="E242" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>96</v>
+      </c>
+      <c r="C243">
+        <v>3.1</v>
+      </c>
+      <c r="D243" t="s">
+        <v>449</v>
+      </c>
+      <c r="E243" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>96</v>
+      </c>
+      <c r="C244">
+        <v>3.2</v>
+      </c>
+      <c r="D244" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>96</v>
+      </c>
+      <c r="C245">
+        <v>3.3</v>
+      </c>
+      <c r="D245" t="s">
+        <v>448</v>
+      </c>
+      <c r="E245" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>96</v>
+      </c>
+      <c r="C246">
+        <v>3.4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>96</v>
+      </c>
+      <c r="C247">
+        <v>3.5</v>
+      </c>
+      <c r="D247" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>96</v>
+      </c>
+      <c r="C248">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D248" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>96</v>
+      </c>
+      <c r="C249">
+        <v>4.2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>96</v>
+      </c>
+      <c r="C250">
+        <v>4.3</v>
+      </c>
+      <c r="D250" t="s">
+        <v>447</v>
+      </c>
+      <c r="E250" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>96</v>
+      </c>
+      <c r="C251" t="s">
+        <v>386</v>
+      </c>
+      <c r="D251" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>96</v>
+      </c>
+      <c r="C252">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D252" t="s">
+        <v>445</v>
+      </c>
+      <c r="E252" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>96</v>
+      </c>
+      <c r="C253">
+        <v>4.5</v>
+      </c>
+      <c r="D253" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>96</v>
+      </c>
+      <c r="C254">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D254" t="s">
+        <v>444</v>
+      </c>
+      <c r="E254" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>96</v>
+      </c>
+      <c r="C255">
+        <v>4.7</v>
+      </c>
+      <c r="D255" t="s">
+        <v>443</v>
+      </c>
+      <c r="E255" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>97</v>
+      </c>
+      <c r="C256">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D256" t="s">
+        <v>442</v>
+      </c>
+      <c r="E256" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>97</v>
+      </c>
+      <c r="C257" t="s">
+        <v>184</v>
+      </c>
+      <c r="D257" t="s">
+        <v>441</v>
+      </c>
+      <c r="E257" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>97</v>
+      </c>
+      <c r="C258">
+        <v>1.2</v>
+      </c>
+      <c r="D258" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>97</v>
+      </c>
+      <c r="C259">
+        <v>1.3</v>
+      </c>
+      <c r="D259" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>97</v>
+      </c>
+      <c r="C260">
+        <v>1.4</v>
+      </c>
+      <c r="D260" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>90</v>
+      </c>
+      <c r="B261">
+        <v>97</v>
+      </c>
+      <c r="C261">
+        <v>2.1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>88</v>
+      </c>
+      <c r="B262">
+        <v>97</v>
+      </c>
+      <c r="C262">
+        <v>3.1</v>
+      </c>
+      <c r="D262" t="s">
+        <v>440</v>
+      </c>
+      <c r="E262" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>88</v>
+      </c>
+      <c r="B263">
+        <v>97</v>
+      </c>
+      <c r="C263">
+        <v>3.2</v>
+      </c>
+      <c r="D263" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>88</v>
+      </c>
+      <c r="B264">
+        <v>97</v>
+      </c>
+      <c r="C264">
+        <v>3.3</v>
+      </c>
+      <c r="D264" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>88</v>
+      </c>
+      <c r="B265">
+        <v>97</v>
+      </c>
+      <c r="C265">
+        <v>3.4</v>
+      </c>
+      <c r="D265" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>90</v>
+      </c>
+      <c r="B266">
+        <v>98</v>
+      </c>
+      <c r="C266">
+        <v>2.1</v>
+      </c>
+      <c r="D266" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>90</v>
+      </c>
+      <c r="B267">
+        <v>99</v>
+      </c>
+      <c r="C267">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D267" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>88</v>
+      </c>
+      <c r="B268">
+        <v>99</v>
+      </c>
+      <c r="C268">
+        <v>2.1</v>
+      </c>
+      <c r="D268" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>88</v>
+      </c>
+      <c r="B269">
+        <v>99</v>
+      </c>
+      <c r="C269">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D269" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>88</v>
+      </c>
+      <c r="B270">
+        <v>99</v>
+      </c>
+      <c r="C270">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D270" t="s">
+        <v>439</v>
+      </c>
+      <c r="E270" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>88</v>
+      </c>
+      <c r="B271">
+        <v>99</v>
+      </c>
+      <c r="C271" t="s">
+        <v>70</v>
+      </c>
+      <c r="D271" t="s">
+        <v>438</v>
+      </c>
+      <c r="E271" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>88</v>
+      </c>
+      <c r="B272">
+        <v>99</v>
+      </c>
+      <c r="C272" t="s">
+        <v>424</v>
+      </c>
+      <c r="D272" t="s">
+        <v>437</v>
+      </c>
+      <c r="E272" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>88</v>
+      </c>
+      <c r="B273">
+        <v>99</v>
+      </c>
+      <c r="C273" t="s">
+        <v>425</v>
+      </c>
+      <c r="D273" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>88</v>
+      </c>
+      <c r="B274">
+        <v>99</v>
+      </c>
+      <c r="C274" t="s">
+        <v>426</v>
+      </c>
+      <c r="D274" t="s">
+        <v>436</v>
+      </c>
+      <c r="E274" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>88</v>
+      </c>
+      <c r="B275">
+        <v>99</v>
+      </c>
+      <c r="C275" t="s">
+        <v>427</v>
+      </c>
+      <c r="D275" t="s">
+        <v>435</v>
+      </c>
+      <c r="E275" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>88</v>
+      </c>
+      <c r="B276">
+        <v>99</v>
+      </c>
+      <c r="C276" t="s">
+        <v>428</v>
+      </c>
+      <c r="D276" t="s">
+        <v>434</v>
+      </c>
+      <c r="E276" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>88</v>
+      </c>
+      <c r="B277">
+        <v>99</v>
+      </c>
+      <c r="C277" t="s">
+        <v>429</v>
+      </c>
+      <c r="D277" t="s">
+        <v>433</v>
+      </c>
+      <c r="E277" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>88</v>
+      </c>
+      <c r="B278">
+        <v>99</v>
+      </c>
+      <c r="C278" t="s">
+        <v>430</v>
+      </c>
+      <c r="D278" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -4175,7 +5790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EAAF48-E021-47AA-8DD6-3DE7D83190CB}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -4191,442 +5806,442 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" t="s">
         <v>263</v>
       </c>
-      <c r="B5" t="s">
-        <v>266</v>
-      </c>
       <c r="C5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C9" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" t="s">
         <v>271</v>
       </c>
-      <c r="B12" t="s">
-        <v>274</v>
-      </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D13" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C14" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C15" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C16" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D16" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" t="s">
         <v>277</v>
       </c>
-      <c r="B17" t="s">
-        <v>280</v>
-      </c>
       <c r="C17" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D18" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C19" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C20" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D20" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D21" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B23" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C23" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D23" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B24" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C24" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D24" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C25" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D25" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B26" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B27" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C27" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" t="s">
         <v>294</v>
       </c>
-      <c r="B28" t="s">
-        <v>297</v>
-      </c>
       <c r="C28" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B29" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C29" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C30" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B31" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C31" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>